<commit_message>
add cases expected for nj
</commit_message>
<xml_diff>
--- a/nj_predictions_2011.xlsx
+++ b/nj_predictions_2011.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gweny\OneDrive\Desktop\CSCI499\FinalProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_895BE7B091E6E8BF891C87C94AEE5E8F7135FEB6" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{FF4C4FB0-74F9-4315-922B-948DCEBC8C5A}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>34001</t>
   </si>
@@ -77,13 +90,25 @@
   </si>
   <si>
     <t>34041</t>
+  </si>
+  <si>
+    <t>fips</t>
+  </si>
+  <si>
+    <t>cases per person</t>
+  </si>
+  <si>
+    <t>total_pop</t>
+  </si>
+  <si>
+    <t>cases_expected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,17 +160,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -192,7 +226,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,9 +258,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,6 +310,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,190 +503,346 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.00469970703125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>4.69970703125E-3</v>
+      </c>
+      <c r="C2">
+        <v>270991</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>1273.5783081054688</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.002128958702087402</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>2.1289587020874019E-3</v>
+      </c>
+      <c r="C3">
+        <v>939151</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D22" si="0">B3*C3</f>
+        <v>1999.4136940240855</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.003558635711669922</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>3.5586357116699219E-3</v>
+      </c>
+      <c r="C4">
+        <v>449284</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1598.8380870819092</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.005830645561218262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>5.8306455612182617E-3</v>
+      </c>
+      <c r="C5">
+        <v>510150</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2974.5038330554962</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.003202080726623535</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>3.2020807266235352E-3</v>
+      </c>
+      <c r="C6">
+        <v>94430</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>302.37248301506042</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.006942510604858398</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>6.9425106048583976E-3</v>
+      </c>
+      <c r="C7">
+        <v>153797</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1067.7373034954069</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.007010698318481445</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>7.0106983184814453E-3</v>
+      </c>
+      <c r="C8">
+        <v>796914</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>5586.9236397743225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.003009915351867676</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>3.0099153518676762E-3</v>
+      </c>
+      <c r="C9">
+        <v>292330</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>879.88855481147777</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.004501104354858398</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>4.5011043548583976E-3</v>
+      </c>
+      <c r="C10">
+        <v>677983</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3051.6722338199611</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.001663565635681152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>1.6635656356811519E-3</v>
+      </c>
+      <c r="C11">
+        <v>124676</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>207.40670919418329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.004777789115905762</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>4.7777891159057617E-3</v>
+      </c>
+      <c r="C12">
+        <v>371023</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1772.6696511507034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.00321507453918457</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>3.2150745391845699E-3</v>
+      </c>
+      <c r="C13">
+        <v>837073</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2691.2520897388454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.002535343170166016</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>2.5353431701660161E-3</v>
+      </c>
+      <c r="C14">
+        <v>625846</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1586.7343816757204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.001748085021972656</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>1.748085021972656E-3</v>
+      </c>
+      <c r="C15">
+        <v>498423</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>871.28578090667713</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.001517176628112793</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>1.517176628112793E-3</v>
+      </c>
+      <c r="C16">
+        <v>592497</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>898.9226006269455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.004940032958984375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>4.940032958984375E-3</v>
+      </c>
+      <c r="C17">
+        <v>507945</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>2509.2650413513184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.003655910491943359</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>3.6559104919433589E-3</v>
+      </c>
+      <c r="C18">
+        <v>63436</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>231.91633796691892</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.002286553382873535</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>2.2865533828735352E-3</v>
+      </c>
+      <c r="C19">
+        <v>333751</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>763.13947808742523</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.001586318016052246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>1.5863180160522461E-3</v>
+      </c>
+      <c r="C20">
+        <v>142522</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>226.08521628379822</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.003930926322937012</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>3.9309263229370117E-3</v>
+      </c>
+      <c r="C21">
+        <v>555630</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>2184.1405928134918</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.002004265785217285</v>
+        <v>2.0042657852172852E-3</v>
+      </c>
+      <c r="C22">
+        <v>106671</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>213.79703557491302</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>